<commit_message>
updated data - 1x and S seem to be working!
</commit_message>
<xml_diff>
--- a/tests/data1.xlsx
+++ b/tests/data1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t xml:space="preserve">SF-RAS(1x)</t>
   </si>
   <si>
-    <t xml:space="preserve">GS Energy</t>
+    <t xml:space="preserve">State 1</t>
   </si>
   <si>
     <t xml:space="preserve">#dets</t>
@@ -37,10 +37,13 @@
     <t xml:space="preserve">N2</t>
   </si>
   <si>
+    <t xml:space="preserve">SF-XCIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Psi4 (1x)</t>
   </si>
   <si>
-    <t xml:space="preserve">SF-XCIS</t>
+    <t xml:space="preserve">Psi4 (S)</t>
   </si>
 </sst>
 </file>
@@ -55,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -76,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,15 +151,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,7 +178,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-149.609461127003</v>
+        <v>-149.562132347448</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>108</v>
@@ -200,10 +205,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>-149.562132340033</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>108</v>
+        <v>-149.604321051649</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,7 +218,31 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>-149.663268056593</v>
+        <v>-149.562132340033</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>-108.780110348207</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>-149.604321051363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>